<commit_message>
Changed 95% Hausdorff distance into Frame of reference
</commit_message>
<xml_diff>
--- a/tests/test_load_existing_dataframe/test_dataframe.xlsx
+++ b/tests/test_load_existing_dataframe/test_dataframe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\università\Magistrale\software_and_computing\tests\test_load_existing_dataframe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Desktop\università\Magistrale\software_and_computing\project\tests\test_load_existing_dataframe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BE3953-31B9-4F49-A050-E16B7CF35A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB3A0A5-DD20-4D7B-AECA-65D32A900D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,10 @@
     <t>Alias name</t>
   </si>
   <si>
-    <t>95% Hausdorff distance (mm)</t>
+    <t>Prostate</t>
   </si>
   <si>
-    <t>Prostate</t>
+    <t>Frame of reference</t>
   </si>
 </sst>
 </file>
@@ -386,14 +386,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -404,7 +404,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>8</v>

</xml_diff>